<commit_message>
Auto-upload VRF Excel file
</commit_message>
<xml_diff>
--- a/vrf_models.xlsx
+++ b/vrf_models.xlsx
@@ -35,7 +35,6 @@
     <sheet name="HNB HEAD OFFICE" sheetId="27" state="visible" r:id="rId27"/>
     <sheet name="Sheet4" sheetId="28" state="visible" r:id="rId28"/>
     <sheet name="Mrs . Rohini" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="cat" sheetId="30" state="visible" r:id="rId30"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -7139,57 +7138,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Outdoor Model</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Outdoor Quantity</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Outdoor Serial(s)</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Indoor Model</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Indoor Quantity</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>Indoor Serial(s)</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>